<commit_message>
updating api to twse
</commit_message>
<xml_diff>
--- a/Data/ana/anaKplot/TAIEX/202508/欄位對照.xlsx
+++ b/Data/ana/anaKplot/TAIEX/202508/欄位對照.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Han\學習\金融策略\Invest\Data\ana\anaKplot\TAIEX\202508\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{305F7D47-6D7F-4DE8-A97D-315D00A4BF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E0B56B-0FFD-47EC-9CED-8B0166AF76C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15890" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{83F67796-42B1-4A79-BEE9-C122C086351D}"/>
   </bookViews>
@@ -16,12 +16,12 @@
     <sheet name="對照" sheetId="3" r:id="rId1"/>
     <sheet name="memo" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="108">
   <si>
     <t>date</t>
   </si>
@@ -400,6 +400,9 @@
   <si>
     <t>買超-自營商(億)</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>跳空缺口</t>
   </si>
 </sst>
 </file>
@@ -1267,10 +1270,10 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="40" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1651,9 +1654,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD981BB-11D9-492C-8A62-AC91570B1CE7}">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -1713,11 +1716,11 @@
         <v>0</v>
       </c>
       <c r="C2" t="str">
-        <f>VLOOKUP(B2,J:K,2,FALSE)</f>
+        <f t="shared" ref="C2:C32" si="0">VLOOKUP(B2,J:K,2,FALSE)</f>
         <v>日期</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D32" si="0">_xlfn.IFNA(""""&amp;A2&amp;""" : """&amp;C2&amp;""",","")</f>
+        <f t="shared" ref="D2:D32" si="1">_xlfn.IFNA(""""&amp;A2&amp;""" : """&amp;C2&amp;""",","")</f>
         <v>"date" : "日期",</v>
       </c>
       <c r="E2" s="21" t="s">
@@ -1752,11 +1755,11 @@
         <v>1</v>
       </c>
       <c r="C3" t="str">
-        <f>VLOOKUP(B3,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>股票代號</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"stock_id" : "股票代號",</v>
       </c>
       <c r="E3" s="21" t="s">
@@ -1766,7 +1769,7 @@
         <v>33</v>
       </c>
       <c r="G3" s="22" t="str">
-        <f t="shared" ref="G3:G14" si="1">VLOOKUP(F3,J:K,2,FALSE)</f>
+        <f t="shared" ref="G3:G14" si="2">VLOOKUP(F3,J:K,2,FALSE)</f>
         <v>5日最大量</v>
       </c>
       <c r="H3" s="22" t="s">
@@ -1779,7 +1782,7 @@
         <v>56</v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" ref="L3:L40" si="2">""""&amp;K3&amp;""","</f>
+        <f t="shared" ref="L3:L40" si="3">""""&amp;K3&amp;""","</f>
         <v>"股票代號",</v>
       </c>
     </row>
@@ -1791,11 +1794,11 @@
         <v>31</v>
       </c>
       <c r="C4" t="str">
-        <f>VLOOKUP(B4,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>成交量</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"Trading_Volume" : "成交量",</v>
       </c>
       <c r="E4" s="21" t="s">
@@ -1805,7 +1808,7 @@
         <v>34</v>
       </c>
       <c r="G4" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10日最大量_日期</v>
       </c>
       <c r="H4" s="22" t="s">
@@ -1818,7 +1821,7 @@
         <v>57</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"開盤價",</v>
       </c>
     </row>
@@ -1830,11 +1833,11 @@
         <v>3</v>
       </c>
       <c r="C5" t="str">
-        <f>VLOOKUP(B5,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>量增率(%)</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"Volume_Change" : "量增率(%)",</v>
       </c>
       <c r="E5" s="21" t="s">
@@ -1844,7 +1847,7 @@
         <v>35</v>
       </c>
       <c r="G5" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10日最大量</v>
       </c>
       <c r="H5" s="22" t="s">
@@ -1857,7 +1860,7 @@
         <v>58</v>
       </c>
       <c r="L5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"收盤價",</v>
       </c>
     </row>
@@ -1869,11 +1872,11 @@
         <v>4</v>
       </c>
       <c r="C6" t="str">
-        <f>VLOOKUP(B6,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>總成交金額(億)</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"Trading_money" : "總成交金額(億)",</v>
       </c>
       <c r="E6" s="21" t="s">
@@ -1883,7 +1886,7 @@
         <v>36</v>
       </c>
       <c r="G6" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20日最大量_日期</v>
       </c>
       <c r="H6" s="22" t="s">
@@ -1896,7 +1899,7 @@
         <v>59</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"收盤-開盤",</v>
       </c>
     </row>
@@ -1908,11 +1911,11 @@
         <v>5</v>
       </c>
       <c r="C7" t="str">
-        <f>VLOOKUP(B7,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>開盤價</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"open" : "開盤價",</v>
       </c>
       <c r="E7" s="21" t="s">
@@ -1922,7 +1925,7 @@
         <v>37</v>
       </c>
       <c r="G7" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20日最大量</v>
       </c>
       <c r="H7" s="22" t="s">
@@ -1935,7 +1938,7 @@
         <v>60</v>
       </c>
       <c r="L7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"最高價",</v>
       </c>
     </row>
@@ -1947,11 +1950,11 @@
         <v>6</v>
       </c>
       <c r="C8" t="str">
-        <f>VLOOKUP(B8,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>最高價</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"max" : "最高價",</v>
       </c>
       <c r="E8" s="21" t="s">
@@ -1961,7 +1964,7 @@
         <v>38</v>
       </c>
       <c r="G8" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>實體(漲跌率)</v>
       </c>
       <c r="H8" s="22" t="s">
@@ -1974,7 +1977,7 @@
         <v>61</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"最低價",</v>
       </c>
     </row>
@@ -1986,11 +1989,11 @@
         <v>7</v>
       </c>
       <c r="C9" t="str">
-        <f>VLOOKUP(B9,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>最低價</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"min" : "最低價",</v>
       </c>
       <c r="E9" s="21" t="s">
@@ -2000,7 +2003,7 @@
         <v>39</v>
       </c>
       <c r="G9" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>上影(%)</v>
       </c>
       <c r="H9" s="22"/>
@@ -2011,7 +2014,7 @@
         <v>62</v>
       </c>
       <c r="L9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"日振幅",</v>
       </c>
     </row>
@@ -2023,11 +2026,11 @@
         <v>8</v>
       </c>
       <c r="C10" t="str">
-        <f>VLOOKUP(B10,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>收盤價</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"close" : "收盤價",</v>
       </c>
       <c r="E10" s="21" t="s">
@@ -2037,7 +2040,7 @@
         <v>40</v>
       </c>
       <c r="G10" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>上影/實體</v>
       </c>
       <c r="H10" s="22"/>
@@ -2048,7 +2051,7 @@
         <v>63</v>
       </c>
       <c r="L10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"成交量",</v>
       </c>
     </row>
@@ -2060,11 +2063,11 @@
         <v>9</v>
       </c>
       <c r="C11" t="str">
-        <f>VLOOKUP(B11,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>收盤-開盤</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"close-open" : "收盤-開盤",</v>
       </c>
       <c r="E11" s="21" t="s">
@@ -2074,7 +2077,7 @@
         <v>41</v>
       </c>
       <c r="G11" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>下影(%)</v>
       </c>
       <c r="H11" s="22"/>
@@ -2085,7 +2088,7 @@
         <v>64</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"量增率(%)",</v>
       </c>
     </row>
@@ -2097,11 +2100,11 @@
         <v>10</v>
       </c>
       <c r="C12" t="str">
-        <f>VLOOKUP(B12,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>日振幅</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"max-min" : "日振幅",</v>
       </c>
       <c r="E12" s="21" t="s">
@@ -2111,7 +2114,7 @@
         <v>42</v>
       </c>
       <c r="G12" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>下影/實體</v>
       </c>
       <c r="H12" s="22"/>
@@ -2122,7 +2125,7 @@
         <v>66</v>
       </c>
       <c r="L12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"5日均量",</v>
       </c>
     </row>
@@ -2134,22 +2137,22 @@
         <v>11</v>
       </c>
       <c r="C13" t="str">
-        <f>VLOOKUP(B13,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>5日均量</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"近5日均量" : "5日均量",</v>
       </c>
       <c r="E13" s="21" t="s">
         <v>95</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="G13" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>跳空率</v>
+        <f t="shared" si="2"/>
+        <v>跳空缺口</v>
       </c>
       <c r="H13" s="22"/>
       <c r="J13" s="5" t="s">
@@ -2159,7 +2162,7 @@
         <v>68</v>
       </c>
       <c r="L13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"5日最大量_日期",</v>
       </c>
     </row>
@@ -2171,7 +2174,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="str">
-        <f>VLOOKUP(B14,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>10日均量</v>
       </c>
       <c r="D14" t="str">
@@ -2185,7 +2188,7 @@
         <v>106</v>
       </c>
       <c r="G14" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>買超-自營商(億)</v>
       </c>
       <c r="H14" s="22" t="s">
@@ -2210,11 +2213,11 @@
         <v>13</v>
       </c>
       <c r="C15" t="str">
-        <f>VLOOKUP(B15,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>20日均量</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"近20日均量" : "20日均量",</v>
       </c>
       <c r="J15" s="5" t="s">
@@ -2224,7 +2227,7 @@
         <v>69</v>
       </c>
       <c r="L15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"10日均量",</v>
       </c>
     </row>
@@ -2236,11 +2239,11 @@
         <v>14</v>
       </c>
       <c r="C16" t="str">
-        <f>VLOOKUP(B16,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>5日平均</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"5MA" : "5日平均",</v>
       </c>
       <c r="J16" s="5" t="s">
@@ -2250,7 +2253,7 @@
         <v>70</v>
       </c>
       <c r="L16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"10日最大量_日期",</v>
       </c>
     </row>
@@ -2262,11 +2265,11 @@
         <v>15</v>
       </c>
       <c r="C17" t="str">
-        <f>VLOOKUP(B17,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>10日平均</v>
       </c>
       <c r="D17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"10MA" : "10日平均",</v>
       </c>
       <c r="J17" s="5" t="s">
@@ -2276,7 +2279,7 @@
         <v>71</v>
       </c>
       <c r="L17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"10日最大量",</v>
       </c>
     </row>
@@ -2288,11 +2291,11 @@
         <v>16</v>
       </c>
       <c r="C18" t="str">
-        <f>VLOOKUP(B18,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>20日平均</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"20MA" : "20日平均",</v>
       </c>
       <c r="J18" s="5" t="s">
@@ -2302,7 +2305,7 @@
         <v>72</v>
       </c>
       <c r="L18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"20日均量",</v>
       </c>
     </row>
@@ -2314,11 +2317,11 @@
         <v>17</v>
       </c>
       <c r="C19" t="str">
-        <f>VLOOKUP(B19,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>5日乖離</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"5_Devi" : "5日乖離",</v>
       </c>
       <c r="J19" s="5" t="s">
@@ -2328,7 +2331,7 @@
         <v>73</v>
       </c>
       <c r="L19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"20日最大量_日期",</v>
       </c>
     </row>
@@ -2340,11 +2343,11 @@
         <v>18</v>
       </c>
       <c r="C20" t="str">
-        <f>VLOOKUP(B20,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>10日乖離</v>
       </c>
       <c r="D20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"10_Devi" : "10日乖離",</v>
       </c>
       <c r="J20" s="5" t="s">
@@ -2354,7 +2357,7 @@
         <v>74</v>
       </c>
       <c r="L20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"20日最大量",</v>
       </c>
     </row>
@@ -2366,7 +2369,7 @@
         <v>19</v>
       </c>
       <c r="C21" t="str">
-        <f>VLOOKUP(B21,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>20日乖離</v>
       </c>
       <c r="D21" t="str">
@@ -2380,7 +2383,7 @@
         <v>38</v>
       </c>
       <c r="L21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"實體(漲跌率)",</v>
       </c>
     </row>
@@ -2392,11 +2395,11 @@
         <v>51</v>
       </c>
       <c r="C22" t="e">
-        <f>VLOOKUP(B22,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="D22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J22" s="6" t="s">
@@ -2406,7 +2409,7 @@
         <v>39</v>
       </c>
       <c r="L22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"上影(%)",</v>
       </c>
     </row>
@@ -2418,11 +2421,11 @@
         <v>99</v>
       </c>
       <c r="C23" t="str">
-        <f>VLOOKUP(B23,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>法人總買超(億)</v>
       </c>
       <c r="D23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"法人總買超" : "法人總買超(億)",</v>
       </c>
       <c r="J23" s="6" t="s">
@@ -2444,11 +2447,11 @@
         <v>100</v>
       </c>
       <c r="C24" t="str">
-        <f>VLOOKUP(B24,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>買超-外資(億)</v>
       </c>
       <c r="D24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"買超-外資" : "買超-外資(億)",</v>
       </c>
       <c r="J24" s="6" t="s">
@@ -2458,7 +2461,7 @@
         <v>41</v>
       </c>
       <c r="L24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"下影(%)",</v>
       </c>
     </row>
@@ -2470,11 +2473,11 @@
         <v>51</v>
       </c>
       <c r="C25" t="e">
-        <f>VLOOKUP(B25,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="D25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J25" s="6" t="s">
@@ -2484,7 +2487,7 @@
         <v>42</v>
       </c>
       <c r="L25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"下影/實體",</v>
       </c>
     </row>
@@ -2496,22 +2499,22 @@
         <v>102</v>
       </c>
       <c r="C26" t="str">
-        <f>VLOOKUP(B26,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>買超-投信(億)</v>
       </c>
       <c r="D26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"買超-投信" : "買超-投信(億)",</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="K26" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="L26" t="str">
-        <f t="shared" si="2"/>
-        <v>"跳空率",</v>
+        <f t="shared" si="3"/>
+        <v>"跳空缺口",</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -2522,11 +2525,11 @@
         <v>51</v>
       </c>
       <c r="C27" t="e">
-        <f>VLOOKUP(B27,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="D27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J27" s="8" t="s">
@@ -2536,7 +2539,7 @@
         <v>75</v>
       </c>
       <c r="L27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"5日平均",</v>
       </c>
     </row>
@@ -2548,11 +2551,11 @@
         <v>51</v>
       </c>
       <c r="C28" t="e">
-        <f>VLOOKUP(B28,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="D28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J28" s="8" t="s">
@@ -2562,7 +2565,7 @@
         <v>76</v>
       </c>
       <c r="L28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"10日平均",</v>
       </c>
     </row>
@@ -2574,11 +2577,11 @@
         <v>51</v>
       </c>
       <c r="C29" t="e">
-        <f>VLOOKUP(B29,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="D29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J29" s="8" t="s">
@@ -2588,7 +2591,7 @@
         <v>77</v>
       </c>
       <c r="L29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"20日平均",</v>
       </c>
     </row>
@@ -2600,11 +2603,11 @@
         <v>48</v>
       </c>
       <c r="C30" t="str">
-        <f>VLOOKUP(B30,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>買超-融資(億)</v>
       </c>
       <c r="D30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"融資增減(億)" : "買超-融資(億)",</v>
       </c>
       <c r="J30" s="8" t="s">
@@ -2614,7 +2617,7 @@
         <v>78</v>
       </c>
       <c r="L30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"5日乖離",</v>
       </c>
     </row>
@@ -2626,11 +2629,11 @@
         <v>29</v>
       </c>
       <c r="C31" t="str">
-        <f>VLOOKUP(B31,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>資金走向</v>
       </c>
       <c r="D31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"資金走向" : "資金走向",</v>
       </c>
       <c r="J31" s="8" t="s">
@@ -2640,7 +2643,7 @@
         <v>79</v>
       </c>
       <c r="L31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"10日乖離",</v>
       </c>
     </row>
@@ -2652,11 +2655,11 @@
         <v>30</v>
       </c>
       <c r="C32" t="str">
-        <f>VLOOKUP(B32,J:K,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>資金走向判讀</v>
       </c>
       <c r="D32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"資金走向判讀" : "資金走向判讀",</v>
       </c>
       <c r="J32" s="8" t="s">
@@ -2666,7 +2669,7 @@
         <v>80</v>
       </c>
       <c r="L32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"20日乖離",</v>
       </c>
     </row>
@@ -2690,7 +2693,7 @@
         <v>44</v>
       </c>
       <c r="L34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"法人總買超(億)",</v>
       </c>
     </row>
@@ -2702,7 +2705,7 @@
         <v>45</v>
       </c>
       <c r="L35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"買超-外資(億)",</v>
       </c>
     </row>
@@ -2714,7 +2717,7 @@
         <v>46</v>
       </c>
       <c r="L36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"買超-投信(億)",</v>
       </c>
     </row>
@@ -2726,7 +2729,7 @@
         <v>47</v>
       </c>
       <c r="L37" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"買超-自營商(億)",</v>
       </c>
     </row>
@@ -2738,7 +2741,7 @@
         <v>48</v>
       </c>
       <c r="L38" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"買超-融資(億)",</v>
       </c>
     </row>
@@ -2750,7 +2753,7 @@
         <v>29</v>
       </c>
       <c r="L39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"資金走向",</v>
       </c>
     </row>
@@ -2762,7 +2765,7 @@
         <v>30</v>
       </c>
       <c r="L40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"資金走向判讀",</v>
       </c>
     </row>

</xml_diff>